<commit_message>
Added numerical output and xCp plot
</commit_message>
<xml_diff>
--- a/HW3/Kuethe & Chow comparison.xlsx
+++ b/HW3/Kuethe & Chow comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eden\Documents\GitHub\AerodynamicsOfWingsAndBodies\HW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AFE1DB1-7CCE-420E-B0A8-AE64ED7CCE82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C502AB7C-5A9D-4CE4-8049-77B40DE5C47D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="11244" xr2:uid="{D95B76FB-2977-407C-9200-85609EFB3EE8}"/>
   </bookViews>
@@ -464,10 +464,10 @@
         <v>0.62656641604010022</v>
       </c>
       <c r="C2">
-        <v>2.5821955438912796</v>
+        <v>2.579353533977641</v>
       </c>
       <c r="D2">
-        <v>3.1211840880504824</v>
+        <v>3.1166482402283155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -478,10 +478,10 @@
         <v>1.6442007079554557</v>
       </c>
       <c r="C3">
-        <v>1.2717956333283409</v>
+        <v>1.2703958726453837</v>
       </c>
       <c r="D3">
-        <v>0.22649611621332785</v>
+        <v>0.22734744821688707</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,10 +492,10 @@
         <v>1.2797845128284628</v>
       </c>
       <c r="C4">
-        <v>0.93718255411882778</v>
+        <v>0.93615107448669987</v>
       </c>
       <c r="D4">
-        <v>0.26770284784306969</v>
+        <v>0.26850882699173761</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,10 +506,10 @@
         <v>1.0537038472469835</v>
       </c>
       <c r="C5">
-        <v>0.76547254472383985</v>
+        <v>0.76463005215356539</v>
       </c>
       <c r="D5">
-        <v>0.27354109342601984</v>
+        <v>0.27434064689873011</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,10 +520,10 @@
         <v>0.89356122264423943</v>
       </c>
       <c r="C6">
-        <v>0.65446023081887528</v>
+        <v>0.6537399203573111</v>
       </c>
       <c r="D6">
-        <v>0.267582103795656</v>
+        <v>0.26838821583734984</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,10 +534,10 @@
         <v>0.77580549311422886</v>
       </c>
       <c r="C7">
-        <v>0.57350656955790702</v>
+        <v>0.57287535812232204</v>
       </c>
       <c r="D7">
-        <v>0.26075984941052172</v>
+        <v>0.26157347014559945</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,10 +548,10 @@
         <v>0.69627677441025237</v>
       </c>
       <c r="C8">
-        <v>0.50997649285542923</v>
+        <v>0.50941520374165705</v>
       </c>
       <c r="D8">
-        <v>0.26756641669201131</v>
+        <v>0.26837254599920757</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -562,10 +562,10 @@
         <v>0.62549414774048528</v>
       </c>
       <c r="C9">
-        <v>0.45764415303027101</v>
+        <v>0.45714046181180162</v>
       </c>
       <c r="D9">
-        <v>0.26834782598134632</v>
+        <v>0.26915309525570946</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -576,10 +576,10 @@
         <v>0.5361341498075084</v>
       </c>
       <c r="C10">
-        <v>0.41302696588187904</v>
+        <v>0.41257238112573447</v>
       </c>
       <c r="D10">
-        <v>0.22962011274571728</v>
+        <v>0.23046800642364804</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -590,10 +590,10 @@
         <v>0.47355502157455492</v>
       </c>
       <c r="C11">
-        <v>0.37396768109929801</v>
+        <v>0.37355608568020626</v>
       </c>
       <c r="D11">
-        <v>0.21029729585409584</v>
+        <v>0.21116645656476302</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -604,10 +604,10 @@
         <v>0.40371547425264187</v>
       </c>
       <c r="C12">
-        <v>0.33901377617869483</v>
+        <v>0.33864065164324308</v>
       </c>
       <c r="D12">
-        <v>0.16026558851558226</v>
+        <v>0.16118981500489993</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -618,10 +618,10 @@
         <v>0.33266155078417692</v>
       </c>
       <c r="C13">
-        <v>0.30711671502298699</v>
+        <v>0.30677869695506654</v>
       </c>
       <c r="D13">
-        <v>7.6789264346822053E-2</v>
+        <v>7.7805366349363803E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -632,10 +632,10 @@
         <v>0.27022453039816036</v>
       </c>
       <c r="C14">
-        <v>0.27746962063942426</v>
+        <v>0.27716423268596124</v>
       </c>
       <c r="D14">
-        <v>2.6811371382859588E-2</v>
+        <v>2.5681244695200812E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -646,10 +646,10 @@
         <v>0.23469756866392788</v>
       </c>
       <c r="C15">
-        <v>0.2494075591293618</v>
+        <v>0.24913305677524808</v>
       </c>
       <c r="D15">
-        <v>6.2676364945636484E-2</v>
+        <v>6.1506764614127331E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -660,10 +660,10 @@
         <v>0.20724491641474821</v>
       </c>
       <c r="C16">
-        <v>0.22233447245093271</v>
+        <v>0.22208976721304097</v>
       </c>
       <c r="D16">
-        <v>7.2810258978736928E-2</v>
+        <v>7.1629505104890245E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -674,10 +674,10 @@
         <v>0.16471591349507789</v>
       </c>
       <c r="C17">
-        <v>0.1956537773492813</v>
+        <v>0.19543843735453054</v>
       </c>
       <c r="D17">
-        <v>0.1878255913332133</v>
+        <v>0.1865182495580229</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -688,10 +688,10 @@
         <v>0.1560990104126295</v>
       </c>
       <c r="C18">
-        <v>0.16867583404614012</v>
+        <v>0.16849018645113747</v>
       </c>
       <c r="D18">
-        <v>8.0569528277375083E-2</v>
+        <v>7.9380234415025133E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -702,10 +702,10 @@
         <v>0.14049298503991939</v>
       </c>
       <c r="C19">
-        <v>0.14044291632028641</v>
+        <v>0.14028834237199356</v>
       </c>
       <c r="D19">
-        <v>3.5637878730209995E-4</v>
+        <v>1.4566041704337329E-3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,10 +716,10 @@
         <v>9.5276851923623493E-2</v>
       </c>
       <c r="C20">
-        <v>0.10926793575464618</v>
+        <v>0.10914767353926497</v>
       </c>
       <c r="D20">
-        <v>0.14684662169818871</v>
+        <v>0.14558438209902969</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -730,10 +730,10 @@
         <v>7.5317158876572867E-3</v>
       </c>
       <c r="C21">
-        <v>7.0899847222243573E-2</v>
+        <v>7.0821813601142078E-2</v>
       </c>
       <c r="D21">
-        <v>8.4135052728730475</v>
+        <v>8.4031446031046375</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +777,10 @@
         <v>1.3936258171201199</v>
       </c>
       <c r="C2">
-        <v>2.9634418990452263</v>
+        <v>2.9601802826755814</v>
       </c>
       <c r="D2">
-        <v>1.1264258042873212</v>
+        <v>1.1240854225797086</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -791,10 +791,10 @@
         <v>1.9550551636824018</v>
       </c>
       <c r="C3">
-        <v>1.4411895006802613</v>
+        <v>1.4396033021221974</v>
       </c>
       <c r="D3">
-        <v>0.2628394699790772</v>
+        <v>0.2636508018471132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -805,10 +805,10 @@
         <v>1.5427357052424877</v>
       </c>
       <c r="C4">
-        <v>1.0491323578783045</v>
+        <v>1.047977664319615</v>
       </c>
       <c r="D4">
-        <v>0.31995327889724212</v>
+        <v>0.32070175030084397</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -819,10 +819,10 @@
         <v>1.2700953414463996</v>
       </c>
       <c r="C5">
-        <v>0.84751498488353516</v>
+        <v>0.84658219495804266</v>
       </c>
       <c r="D5">
-        <v>0.33271546062173957</v>
+        <v>0.33344988574326645</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,10 +833,10 @@
         <v>1.120714156525334</v>
       </c>
       <c r="C6">
-        <v>0.71791861221492881</v>
+        <v>0.71712845834067018</v>
       </c>
       <c r="D6">
-        <v>0.35940970493246366</v>
+        <v>0.36011474989835257</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -847,10 +847,10 @@
         <v>0.99395395705759237</v>
       </c>
       <c r="C7">
-        <v>0.62454027210327279</v>
+        <v>0.62385289207545813</v>
       </c>
       <c r="D7">
-        <v>0.371660761880658</v>
+        <v>0.37235232311740735</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -861,10 +861,10 @@
         <v>0.88009973387075935</v>
       </c>
       <c r="C8">
-        <v>0.55233389775575015</v>
+        <v>0.55172598933581063</v>
       </c>
       <c r="D8">
-        <v>0.37241896969274718</v>
+        <v>0.37310969643262004</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -875,10 +875,10 @@
         <v>0.78509417874583365</v>
       </c>
       <c r="C9">
-        <v>0.4937030335737474</v>
+        <v>0.4931596553159977</v>
       </c>
       <c r="D9">
-        <v>0.37115438257047784</v>
+        <v>0.37184650113721812</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,10 +889,10 @@
         <v>0.7108105314833475</v>
       </c>
       <c r="C10">
-        <v>0.44432380795679843</v>
+        <v>0.44383477734482002</v>
       </c>
       <c r="D10">
-        <v>0.37490542377085218</v>
+        <v>0.37559341387555406</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,10 +903,10 @@
         <v>0.62253572074516184</v>
       </c>
       <c r="C11">
-        <v>0.4015113783602795</v>
+        <v>0.40106946786266523</v>
       </c>
       <c r="D11">
-        <v>0.35503881146020178</v>
+        <v>0.35574866710846131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,10 +917,10 @@
         <v>0.56035707826266701</v>
       </c>
       <c r="C12">
-        <v>0.36347899918185789</v>
+        <v>0.363078947790894</v>
       </c>
       <c r="D12">
-        <v>0.35134396747732816</v>
+        <v>0.35205788973597835</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,10 +931,10 @@
         <v>0.49764876107795258</v>
       </c>
       <c r="C13">
-        <v>0.32896249586576304</v>
+        <v>0.32860043394652594</v>
       </c>
       <c r="D13">
-        <v>0.33896651294137597</v>
+        <v>0.33969405804457858</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,10 +945,10 @@
         <v>0.42793840270780042</v>
       </c>
       <c r="C14">
-        <v>0.29701101515434303</v>
+        <v>0.29668411959775953</v>
       </c>
       <c r="D14">
-        <v>0.30594914297246562</v>
+        <v>0.30671302757481739</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -959,10 +959,10 @@
         <v>0.35634188564193986</v>
       </c>
       <c r="C15">
-        <v>0.26685808323336624</v>
+        <v>0.2665643745249468</v>
       </c>
       <c r="D15">
-        <v>0.25111783378305663</v>
+        <v>0.25194206669042402</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -973,10 +973,10 @@
         <v>0.29121773505929771</v>
       </c>
       <c r="C16">
-        <v>0.23783008716997062</v>
+        <v>0.23756832718548854</v>
       </c>
       <c r="D16">
-        <v>0.18332553777487592</v>
+        <v>0.18422438407772485</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -987,10 +987,10 @@
         <v>0.240071829057179</v>
       </c>
       <c r="C17">
-        <v>0.20926441783071251</v>
+        <v>0.20903409772522891</v>
       </c>
       <c r="D17">
-        <v>0.12832580710304395</v>
+        <v>0.12928518707856262</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,10 +1001,10 @@
         <v>0.18086453246518358</v>
       </c>
       <c r="C18">
-        <v>0.18040667576033026</v>
+        <v>0.18020811699424072</v>
       </c>
       <c r="D18">
-        <v>2.5314897211340124E-3</v>
+        <v>3.6293211388430816E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1015,10 +1015,10 @@
         <v>0.12057204867839702</v>
       </c>
       <c r="C19">
-        <v>0.15022221317411458</v>
+        <v>0.15005687595939374</v>
       </c>
       <c r="D19">
-        <v>0.24591242183172757</v>
+        <v>0.24454114866739868</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,10 +1029,10 @@
         <v>5.7592434694984887E-2</v>
       </c>
       <c r="C20">
-        <v>0.11690214481670978</v>
+        <v>0.11677348025632082</v>
       </c>
       <c r="D20">
-        <v>1.0298177258147683</v>
+        <v>1.0275836726605585</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1043,10 +1043,10 @@
         <v>7.5317158876572867E-3</v>
       </c>
       <c r="C21">
-        <v>7.5894033377447573E-2</v>
+        <v>7.5810503067067533E-2</v>
       </c>
       <c r="D21">
-        <v>9.0765927060286575</v>
+        <v>9.0655022305479065</v>
       </c>
     </row>
   </sheetData>
@@ -1090,10 +1090,10 @@
         <v>1.937834276412681</v>
       </c>
       <c r="C2">
-        <v>3.127845192430454</v>
+        <v>3.1244026308993438</v>
       </c>
       <c r="D2">
-        <v>0.61409323310181163</v>
+        <v>0.61231673364929751</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1104,10 +1104,10 @@
         <v>2.0676950107226828</v>
       </c>
       <c r="C3">
-        <v>1.5237279900343794</v>
+        <v>1.5220509481606097</v>
       </c>
       <c r="D3">
-        <v>0.26307894436432422</v>
+        <v>0.26389001266263362</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,10 +1118,10 @@
         <v>1.5370772291553625</v>
       </c>
       <c r="C4">
-        <v>1.1104521885539063</v>
+        <v>1.1092300053091255</v>
       </c>
       <c r="D4">
-        <v>0.27755602159033377</v>
+        <v>0.27835115616236328</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1132,10 +1132,10 @@
         <v>1.2932330827067668</v>
       </c>
       <c r="C5">
-        <v>0.89751359782409579</v>
+        <v>0.89652577854422932</v>
       </c>
       <c r="D5">
-        <v>0.30599239238020498</v>
+        <v>0.30675622938149705</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1146,10 +1146,10 @@
         <v>1.1476242151771179</v>
       </c>
       <c r="C6">
-        <v>0.76021686475383388</v>
+        <v>0.75938015667754022</v>
       </c>
       <c r="D6">
-        <v>0.33757334962080227</v>
+        <v>0.33830242806410132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1160,10 +1160,10 @@
         <v>1.0126475983773868</v>
       </c>
       <c r="C7">
-        <v>0.66091745817472447</v>
+        <v>0.66019004077495846</v>
       </c>
       <c r="D7">
-        <v>0.34733715931016496</v>
+        <v>0.34805549153248155</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1174,10 +1174,10 @@
         <v>0.88668837041056248</v>
       </c>
       <c r="C8">
-        <v>0.5838336615636851</v>
+        <v>0.58319108394867725</v>
       </c>
       <c r="D8">
-        <v>0.34155710050267923</v>
+        <v>0.34228179435956418</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1188,10 +1188,10 @@
         <v>0.77984910730434331</v>
       </c>
       <c r="C9">
-        <v>0.5210174991775085</v>
+        <v>0.52044405813763694</v>
       </c>
       <c r="D9">
-        <v>0.33189960173388183</v>
+        <v>0.33263492480407642</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1202,10 +1202,10 @@
         <v>0.70125054905304496</v>
       </c>
       <c r="C10">
-        <v>0.46795592686618309</v>
+        <v>0.46744088632773634</v>
       </c>
       <c r="D10">
-        <v>0.33268369272850962</v>
+        <v>0.33341815281434095</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1216,10 +1216,10 @@
         <v>0.62669560499186105</v>
       </c>
       <c r="C11">
-        <v>0.42185363728005842</v>
+        <v>0.42138933773384879</v>
       </c>
       <c r="D11">
-        <v>0.3268603865738981</v>
+        <v>0.32760125589308797</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1230,10 +1230,10 @@
         <v>0.57799137017802238</v>
       </c>
       <c r="C12">
-        <v>0.3808558719252898</v>
+        <v>0.38043669524200541</v>
       </c>
       <c r="D12">
-        <v>0.3410699682107961</v>
+        <v>0.3417951982140664</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1244,10 +1244,10 @@
         <v>0.53384750536134151</v>
       </c>
       <c r="C13">
-        <v>0.34365551464122235</v>
+        <v>0.34327728132663132</v>
       </c>
       <c r="D13">
-        <v>0.35626651583093055</v>
+        <v>0.3569750202461287</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1258,10 +1258,10 @@
         <v>0.45929256130015761</v>
       </c>
       <c r="C14">
-        <v>0.30927483244824489</v>
+        <v>0.30893443911826102</v>
       </c>
       <c r="D14">
-        <v>0.32662782176842814</v>
+        <v>0.32736894705253961</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1272,10 +1272,10 @@
         <v>0.38097821874273308</v>
       </c>
       <c r="C15">
-        <v>0.27693148414245783</v>
+        <v>0.27662668847150523</v>
       </c>
       <c r="D15">
-        <v>0.27310415525496462</v>
+        <v>0.27390418962952401</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1286,10 +1286,10 @@
         <v>0.29174740976151714</v>
       </c>
       <c r="C16">
-        <v>0.24594373463275573</v>
+        <v>0.24567304462491529</v>
       </c>
       <c r="D16">
-        <v>0.15699770964959953</v>
+        <v>0.15792553282397392</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1300,10 +1300,10 @@
         <v>0.21693408779681164</v>
       </c>
       <c r="C17">
-        <v>0.21564565257084448</v>
+        <v>0.21540830916596854</v>
       </c>
       <c r="D17">
-        <v>5.9392935386621279E-3</v>
+        <v>7.0333742674512506E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1314,10 +1314,10 @@
         <v>0.15892824845619202</v>
       </c>
       <c r="C18">
-        <v>0.18528013782310632</v>
+        <v>0.18507621523880111</v>
       </c>
       <c r="D18">
-        <v>0.16580997791703528</v>
+        <v>0.16452686691388707</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1328,10 +1328,10 @@
         <v>0.11142547089372916</v>
       </c>
       <c r="C19">
-        <v>0.15380273129491573</v>
+        <v>0.15363345329886327</v>
       </c>
       <c r="D19">
-        <v>0.38031932969440557</v>
+        <v>0.3788001259190506</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1342,10 +1342,10 @@
         <v>5.3290442601348728E-2</v>
       </c>
       <c r="C20">
-        <v>0.11937190723923631</v>
+        <v>0.11924052441480761</v>
       </c>
       <c r="D20">
-        <v>1.2400246913358368</v>
+        <v>1.237559280691539</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1356,10 +1356,10 @@
         <v>7.5317158876572867E-3</v>
       </c>
       <c r="C21">
-        <v>7.7337853374365953E-2</v>
+        <v>7.725273397025742E-2</v>
       </c>
       <c r="D21">
-        <v>9.2682913864428329</v>
+        <v>9.2569899240167182</v>
       </c>
     </row>
   </sheetData>
@@ -1403,10 +1403,10 @@
         <v>1.7198279203162545</v>
       </c>
       <c r="C2">
-        <v>2.8261773001362762</v>
+        <v>2.8230667596027832</v>
       </c>
       <c r="D2">
-        <v>0.64329074249275942</v>
+        <v>0.64148210774695236</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1417,10 +1417,10 @@
         <v>1.7631578947368423</v>
       </c>
       <c r="C3">
-        <v>1.3442562078704565</v>
+        <v>1.3427766958024134</v>
       </c>
       <c r="D3">
-        <v>0.23758603135705458</v>
+        <v>0.2384251576046014</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1431,10 +1431,10 @@
         <v>1.3494819523034389</v>
       </c>
       <c r="C4">
-        <v>0.95182621325554906</v>
+        <v>0.95077861655415585</v>
       </c>
       <c r="D4">
-        <v>0.29467288419021009</v>
+        <v>0.29544917964166467</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1445,10 +1445,10 @@
         <v>1.0287962173474925</v>
       </c>
       <c r="C5">
-        <v>0.74512132054831781</v>
+        <v>0.74430122689395739</v>
       </c>
       <c r="D5">
-        <v>0.27573477819598058</v>
+        <v>0.27653191726058063</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1459,10 +1459,10 @@
         <v>0.88951760845412498</v>
       </c>
       <c r="C6">
-        <v>0.61004862990005204</v>
+        <v>0.60937719962898695</v>
       </c>
       <c r="D6">
-        <v>0.31418037810376404</v>
+        <v>0.31493520326369762</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1473,10 +1473,10 @@
         <v>0.75198305040952895</v>
       </c>
       <c r="C7">
-        <v>0.51194746339346586</v>
+        <v>0.51138400499478975</v>
       </c>
       <c r="D7">
-        <v>0.31920345396793193</v>
+        <v>0.31995275064206474</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>0.62279409864868351</v>
       </c>
       <c r="C8">
-        <v>0.43622592700316831</v>
+        <v>0.43574580906165084</v>
       </c>
       <c r="D8">
-        <v>0.29956637683357018</v>
+        <v>0.30033728642079849</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,10 +1501,10 @@
         <v>0.5393638736015296</v>
       </c>
       <c r="C9">
-        <v>0.37548258748605634</v>
+        <v>0.37506932473430293</v>
       </c>
       <c r="D9">
-        <v>0.3038417924084868</v>
+        <v>0.30460799639800112</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,10 +1515,10 @@
         <v>0.45081776606464613</v>
       </c>
       <c r="C10">
-        <v>0.32544838400261744</v>
+        <v>0.32509018977681625</v>
       </c>
       <c r="D10">
-        <v>0.27809325962555576</v>
+        <v>0.27888780290393628</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1529,10 +1529,10 @@
         <v>0.38568069658682785</v>
       </c>
       <c r="C11">
-        <v>0.28341061995868233</v>
+        <v>0.28309869323668879</v>
       </c>
       <c r="D11">
-        <v>0.26516773469143945</v>
+        <v>0.2659765040303097</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1543,10 +1543,10 @@
         <v>0.33320414438157248</v>
       </c>
       <c r="C12">
-        <v>0.24751112300086958</v>
+        <v>0.24723870789777377</v>
       </c>
       <c r="D12">
-        <v>0.25717873809687841</v>
+        <v>0.25799630026616482</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1557,10 +1557,10 @@
         <v>0.28394439707516211</v>
       </c>
       <c r="C13">
-        <v>0.21640008990783671</v>
+        <v>0.21616191615593516</v>
       </c>
       <c r="D13">
-        <v>0.2378786405475222</v>
+        <v>0.23871744474424139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1571,10 +1571,10 @@
         <v>0.2497610004392424</v>
       </c>
       <c r="C14">
-        <v>0.18904927038631381</v>
+        <v>0.18884119942829702</v>
       </c>
       <c r="D14">
-        <v>0.24307930359887195</v>
+        <v>0.24391238385419947</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1585,10 +1585,10 @@
         <v>0.20185773712632094</v>
       </c>
       <c r="C15">
-        <v>0.16464091519551005</v>
+        <v>0.16445970850328839</v>
       </c>
       <c r="D15">
-        <v>0.18437154037608625</v>
+        <v>0.18526923543004525</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1599,10 +1599,10 @@
         <v>0.17117536108312018</v>
       </c>
       <c r="C16">
-        <v>0.14249290976240414</v>
+        <v>0.1423360795552088</v>
       </c>
       <c r="D16">
-        <v>0.16756179825896947</v>
+        <v>0.16847799441128361</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1613,10 +1613,10 @@
         <v>0.10335116140867633</v>
       </c>
       <c r="C17">
-        <v>0.12199763350781503</v>
+        <v>0.12186336076279003</v>
       </c>
       <c r="D17">
-        <v>0.18041860241324137</v>
+        <v>0.17911941290056568</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1627,10 +1627,10 @@
         <v>6.1364752086401568E-2</v>
       </c>
       <c r="C18">
-        <v>0.10255466371118398</v>
+        <v>0.10244179024130008</v>
       </c>
       <c r="D18">
-        <v>0.67123079983745415</v>
+        <v>0.66939141377222622</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1641,10 +1641,10 @@
         <v>4.3058677621889779E-2</v>
       </c>
       <c r="C19">
-        <v>8.3461447425852237E-2</v>
+        <v>8.3369588286233073E-2</v>
       </c>
       <c r="D19">
-        <v>0.9383188717208274</v>
+        <v>0.93618552381762876</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1655,10 +1655,10 @@
         <v>1.7763480867116245E-2</v>
       </c>
       <c r="C20">
-        <v>6.3645705738249569E-2</v>
+        <v>6.3575656153083748E-2</v>
       </c>
       <c r="D20">
-        <v>2.5829523624545061</v>
+        <v>2.5790089019531641</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1669,10 +1669,10 @@
         <v>7.5317158876572867E-3</v>
       </c>
       <c r="C21">
-        <v>4.0621962846684054E-2</v>
+        <v>4.0577253598620883E-2</v>
       </c>
       <c r="D21">
-        <v>4.3934539555924976</v>
+        <v>4.3875178251369613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>